<commit_message>
Fixed some issues with interest calculation deduction, sending of SMS when interest accrued is less than 0, withdrawal service charge not added to transaction.
</commit_message>
<xml_diff>
--- a/src/Monivault.Web.Mvc/wwwroot/TransactionHistory_Temp/TransactionHistory_Template.xlsx
+++ b/src/Monivault.Web.Mvc/wwwroot/TransactionHistory_Temp/TransactionHistory_Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Amount</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Transaction Date</t>
+  </si>
+  <si>
+    <t>Balance After Transaction</t>
   </si>
 </sst>
 </file>
@@ -421,18 +424,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="24.09765625" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,6 +449,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>